<commit_message>
Import Price Levels from Excel
</commit_message>
<xml_diff>
--- a/aspnet-core/src/onetouch.Web.Host/Assets/Products.xlsx
+++ b/aspnet-core/src/onetouch.Web.Host/Assets/Products.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="81">
   <si>
     <t>Record Type</t>
   </si>
@@ -250,6 +250,18 @@
   </si>
   <si>
     <t>Dimension3Position</t>
+  </si>
+  <si>
+    <t>Price A</t>
+  </si>
+  <si>
+    <t>Price D</t>
+  </si>
+  <si>
+    <t>Price C</t>
+  </si>
+  <si>
+    <t>Price B</t>
   </si>
 </sst>
 </file>
@@ -664,10 +676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AM993"/>
+  <dimension ref="A1:AQ993"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
-      <selection activeCell="AR1" sqref="AR1"/>
+      <selection activeCell="AM1" sqref="AM1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -689,7 +701,7 @@
     <col min="27" max="16384" width="14.42578125" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="16" customFormat="1" ht="39" thickBot="1">
+    <row r="1" spans="1:43" s="16" customFormat="1" ht="39" thickBot="1">
       <c r="A1" s="16" t="s">
         <v>15</v>
       </c>
@@ -807,50 +819,62 @@
       <c r="AM1" s="16" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="2" spans="1:39">
+      <c r="AN1" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="AO1" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="AP1" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="AQ1" s="16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:43">
       <c r="T2" s="18"/>
     </row>
-    <row r="3" spans="1:39">
+    <row r="3" spans="1:43">
       <c r="T3" s="18"/>
     </row>
-    <row r="4" spans="1:39">
+    <row r="4" spans="1:43">
       <c r="T4" s="18"/>
     </row>
-    <row r="5" spans="1:39">
+    <row r="5" spans="1:43">
       <c r="T5" s="18"/>
     </row>
-    <row r="6" spans="1:39">
+    <row r="6" spans="1:43">
       <c r="T6" s="18"/>
     </row>
-    <row r="7" spans="1:39">
+    <row r="7" spans="1:43">
       <c r="T7" s="18"/>
     </row>
-    <row r="8" spans="1:39">
+    <row r="8" spans="1:43">
       <c r="T8" s="18"/>
     </row>
-    <row r="9" spans="1:39">
+    <row r="9" spans="1:43">
       <c r="T9" s="18"/>
     </row>
-    <row r="10" spans="1:39">
+    <row r="10" spans="1:43">
       <c r="T10" s="18"/>
     </row>
-    <row r="11" spans="1:39">
+    <row r="11" spans="1:43">
       <c r="T11" s="18"/>
     </row>
-    <row r="12" spans="1:39">
+    <row r="12" spans="1:43">
       <c r="T12" s="18"/>
     </row>
-    <row r="13" spans="1:39">
+    <row r="13" spans="1:43">
       <c r="T13" s="18"/>
     </row>
-    <row r="14" spans="1:39" ht="15.75" customHeight="1">
+    <row r="14" spans="1:43" ht="15.75" customHeight="1">
       <c r="T14" s="18"/>
     </row>
-    <row r="15" spans="1:39" ht="15.75" customHeight="1">
+    <row r="15" spans="1:43" ht="15.75" customHeight="1">
       <c r="T15" s="18"/>
     </row>
-    <row r="16" spans="1:39" ht="15.75" customHeight="1">
+    <row r="16" spans="1:43" ht="15.75" customHeight="1">
       <c r="T16" s="18"/>
     </row>
     <row r="17" spans="20:20" ht="15.75" customHeight="1">

</xml_diff>